<commit_message>
added candle stick analysis
</commit_message>
<xml_diff>
--- a/nifty_gap_opening_trading_analysis_report.xlsx
+++ b/nifty_gap_opening_trading_analysis_report.xlsx
@@ -638,7 +638,7 @@
         </is>
       </c>
       <c r="K3" s="10" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="L3" s="2" t="n"/>
       <c r="M3" s="11" t="inlineStr">
@@ -647,7 +647,7 @@
         </is>
       </c>
       <c r="N3" s="10" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" s="18">
@@ -683,7 +683,7 @@
         </is>
       </c>
       <c r="N4" s="10" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1" s="18">
@@ -721,7 +721,7 @@
         </is>
       </c>
       <c r="N5" s="10" t="n">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1" s="18">
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="N6" s="10" t="n">
-        <v>56</v>
+        <v>55.88</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1" s="18">
@@ -844,7 +844,7 @@
         </is>
       </c>
       <c r="N9" s="14" t="n">
-        <v>680</v>
+        <v>920</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1" s="18">
@@ -884,14 +884,20 @@
       <c r="B11" s="3" t="n">
         <v>78.29999999999927</v>
       </c>
-      <c r="C11" s="0" t="inlineStr">
-        <is>
-          <t>No trading</t>
-        </is>
-      </c>
-      <c r="D11" s="3" t="n"/>
-      <c r="E11" s="3" t="n"/>
-      <c r="F11" s="3" t="inlineStr"/>
+      <c r="C11" s="0" t="inlineStr"/>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>09:16:00</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>09:29:00</t>
+        </is>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>-40</v>
+      </c>
       <c r="I11" s="2" t="n"/>
       <c r="J11" s="2" t="n"/>
       <c r="L11" s="2" t="n"/>
@@ -1586,14 +1592,20 @@
       <c r="B41" s="3" t="n">
         <v>70.54999999999927</v>
       </c>
-      <c r="C41" s="0" t="inlineStr">
-        <is>
-          <t>No trading</t>
-        </is>
-      </c>
-      <c r="D41" s="3" t="n"/>
-      <c r="E41" s="3" t="n"/>
-      <c r="F41" s="3" t="inlineStr"/>
+      <c r="C41" s="0" t="inlineStr"/>
+      <c r="D41" s="3" t="inlineStr">
+        <is>
+          <t>09:16:00</t>
+        </is>
+      </c>
+      <c r="E41" s="3" t="inlineStr">
+        <is>
+          <t>09:45:00</t>
+        </is>
+      </c>
+      <c r="F41" s="3" t="n">
+        <v>-40</v>
+      </c>
       <c r="I41" s="2" t="n"/>
       <c r="J41" s="2" t="n"/>
       <c r="L41" s="2" t="n"/>
@@ -1674,14 +1686,20 @@
       <c r="B45" s="3" t="n">
         <v>-72.40000000000146</v>
       </c>
-      <c r="C45" s="8" t="inlineStr">
-        <is>
-          <t>No trading</t>
-        </is>
-      </c>
-      <c r="D45" s="3" t="n"/>
-      <c r="E45" s="3" t="n"/>
-      <c r="F45" s="3" t="inlineStr"/>
+      <c r="C45" s="8" t="inlineStr"/>
+      <c r="D45" s="3" t="inlineStr">
+        <is>
+          <t>09:16:00</t>
+        </is>
+      </c>
+      <c r="E45" s="3" t="inlineStr">
+        <is>
+          <t>10:41:00</t>
+        </is>
+      </c>
+      <c r="F45" s="3" t="n">
+        <v>80</v>
+      </c>
       <c r="I45" s="2" t="n"/>
       <c r="J45" s="2" t="n"/>
       <c r="L45" s="2" t="n"/>
@@ -1812,14 +1830,20 @@
       <c r="B51" s="3" t="n">
         <v>71.79999999999927</v>
       </c>
-      <c r="C51" s="0" t="inlineStr">
-        <is>
-          <t>No trading</t>
-        </is>
-      </c>
-      <c r="D51" s="3" t="n"/>
-      <c r="E51" s="3" t="n"/>
-      <c r="F51" s="3" t="inlineStr"/>
+      <c r="C51" s="0" t="inlineStr"/>
+      <c r="D51" s="3" t="inlineStr">
+        <is>
+          <t>09:16:00</t>
+        </is>
+      </c>
+      <c r="E51" s="3" t="inlineStr">
+        <is>
+          <t>09:43:00</t>
+        </is>
+      </c>
+      <c r="F51" s="3" t="n">
+        <v>80</v>
+      </c>
       <c r="I51" s="2" t="n"/>
       <c r="J51" s="2" t="n"/>
       <c r="L51" s="2" t="n"/>
@@ -2994,14 +3018,20 @@
       <c r="B101" s="3" t="n">
         <v>76.95000000000073</v>
       </c>
-      <c r="C101" s="0" t="inlineStr">
-        <is>
-          <t>No trading</t>
-        </is>
-      </c>
-      <c r="D101" s="3" t="n"/>
-      <c r="E101" s="3" t="n"/>
-      <c r="F101" s="3" t="inlineStr"/>
+      <c r="C101" s="0" t="inlineStr"/>
+      <c r="D101" s="3" t="inlineStr">
+        <is>
+          <t>09:16:00</t>
+        </is>
+      </c>
+      <c r="E101" s="3" t="inlineStr">
+        <is>
+          <t>09:26:00</t>
+        </is>
+      </c>
+      <c r="F101" s="3" t="n">
+        <v>-40</v>
+      </c>
       <c r="I101" s="2" t="n"/>
       <c r="J101" s="2" t="n"/>
       <c r="L101" s="2" t="n"/>
@@ -3132,14 +3162,20 @@
       <c r="B107" s="3" t="n">
         <v>78.95000000000073</v>
       </c>
-      <c r="C107" s="8" t="inlineStr">
-        <is>
-          <t>No trading</t>
-        </is>
-      </c>
-      <c r="D107" s="3" t="n"/>
-      <c r="E107" s="3" t="n"/>
-      <c r="F107" s="3" t="inlineStr"/>
+      <c r="C107" s="8" t="inlineStr"/>
+      <c r="D107" s="3" t="inlineStr">
+        <is>
+          <t>09:16:00</t>
+        </is>
+      </c>
+      <c r="E107" s="3" t="inlineStr">
+        <is>
+          <t>09:36:00</t>
+        </is>
+      </c>
+      <c r="F107" s="3" t="n">
+        <v>80</v>
+      </c>
       <c r="I107" s="2" t="n"/>
       <c r="J107" s="2" t="n"/>
       <c r="L107" s="2" t="n"/>
@@ -3264,14 +3300,20 @@
       <c r="B113" s="3" t="n">
         <v>-78.5</v>
       </c>
-      <c r="C113" s="0" t="inlineStr">
-        <is>
-          <t>No trading</t>
-        </is>
-      </c>
-      <c r="D113" s="3" t="n"/>
-      <c r="E113" s="3" t="n"/>
-      <c r="F113" s="3" t="inlineStr"/>
+      <c r="C113" s="0" t="inlineStr"/>
+      <c r="D113" s="3" t="inlineStr">
+        <is>
+          <t>09:16:00</t>
+        </is>
+      </c>
+      <c r="E113" s="3" t="inlineStr">
+        <is>
+          <t>09:23:00</t>
+        </is>
+      </c>
+      <c r="F113" s="3" t="n">
+        <v>-40</v>
+      </c>
       <c r="I113" s="2" t="n"/>
       <c r="J113" s="2" t="n"/>
       <c r="L113" s="2" t="n"/>
@@ -3286,14 +3328,20 @@
       <c r="B114" s="3" t="n">
         <v>70.54999999999927</v>
       </c>
-      <c r="C114" s="8" t="inlineStr">
-        <is>
-          <t>No trading</t>
-        </is>
-      </c>
-      <c r="D114" s="3" t="n"/>
-      <c r="E114" s="3" t="n"/>
-      <c r="F114" s="3" t="inlineStr"/>
+      <c r="C114" s="8" t="inlineStr"/>
+      <c r="D114" s="3" t="inlineStr">
+        <is>
+          <t>09:16:00</t>
+        </is>
+      </c>
+      <c r="E114" s="3" t="inlineStr">
+        <is>
+          <t>10:18:00</t>
+        </is>
+      </c>
+      <c r="F114" s="3" t="n">
+        <v>80</v>
+      </c>
       <c r="I114" s="2" t="n"/>
       <c r="J114" s="2" t="n"/>
       <c r="L114" s="2" t="n"/>
@@ -3358,14 +3406,20 @@
       <c r="B117" s="3" t="n">
         <v>70</v>
       </c>
-      <c r="C117" s="8" t="inlineStr">
-        <is>
-          <t>No trading</t>
-        </is>
-      </c>
-      <c r="D117" s="3" t="n"/>
-      <c r="E117" s="3" t="n"/>
-      <c r="F117" s="3" t="inlineStr"/>
+      <c r="C117" s="8" t="inlineStr"/>
+      <c r="D117" s="3" t="inlineStr">
+        <is>
+          <t>09:16:00</t>
+        </is>
+      </c>
+      <c r="E117" s="3" t="inlineStr">
+        <is>
+          <t>09:48:00</t>
+        </is>
+      </c>
+      <c r="F117" s="3" t="n">
+        <v>80</v>
+      </c>
       <c r="I117" s="2" t="n"/>
       <c r="J117" s="2" t="n"/>
       <c r="L117" s="2" t="n"/>

</xml_diff>